<commit_message>
Changed format of flavor grouping file to csv
</commit_message>
<xml_diff>
--- a/data/flavorgrouping.xlsx
+++ b/data/flavorgrouping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13800" tabRatio="500"/>
+    <workbookView xWindow="3360" yWindow="5080" windowWidth="25360" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Carbonation</t>
   </si>
@@ -189,18 +189,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -530,139 +555,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I7"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:9">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="B9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="D7" t="s">
-        <v>0</v>
-      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="H14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>